<commit_message>
update agreement and mesInterface
</commit_message>
<xml_diff>
--- a/RetrospectiveSystem/document/追溯系统/FVS MES项目_SMT线烧录 _V0. 1.xlsx
+++ b/RetrospectiveSystem/document/追溯系统/FVS MES项目_SMT线烧录 _V0. 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12015" tabRatio="884" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12465" tabRatio="884" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MES接口清单" sheetId="80" r:id="rId1"/>
@@ -175,8 +175,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -226,8 +226,126 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,113 +358,10 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -358,23 +373,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="DengXian"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="DengXian"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="DengXian"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,13 +419,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,169 +575,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,6 +718,24 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -737,6 +755,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -748,39 +777,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,13 +796,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -816,10 +816,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -828,140 +828,140 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="44">
@@ -1592,7 +1592,7 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1752,8 +1752,8 @@
   <sheetPr/>
   <dimension ref="E1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="14.25" outlineLevelRow="6"/>

</xml_diff>